<commit_message>
test-data: update playwright-data-driven-template.xlsx with new values
</commit_message>
<xml_diff>
--- a/SiemensApplication/test-data/playwright-data-driven-template.xlsx
+++ b/SiemensApplication/test-data/playwright-data-driven-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinee\PlaywrightBolt\playwright-pega-framework\SiemensApplication\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sai12\Desktop\Siemens\Sep 3\playwright-pega-framework-POM 1\playwright-pega-framework-POM\SiemensApplication\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FA2CE4-F4A2-4D37-ABD9-F93A74921C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA3F41-F69D-402E-B5CA-62E4FE67EDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Env" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>key</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>dateISO</t>
-  </si>
-  <si>
-    <t>2025-08-23</t>
   </si>
   <si>
     <t>changeNumber</t>
@@ -409,12 +406,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,14 +723,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,29 +741,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -776,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -800,13 +798,13 @@
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -814,44 +812,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -867,13 +865,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -894,13 +892,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -908,52 +906,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -967,14 +965,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -985,7 +983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1009,13 +1007,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1040,17 +1038,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="69.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1058,23 +1056,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1082,7 +1080,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1090,15 +1088,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1106,7 +1104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1114,7 +1112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1130,15 +1128,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1146,7 +1144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1154,100 +1152,100 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3">
+        <v>45923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1259,36 +1257,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="1" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1296,13 +1294,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1310,13 +1308,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1324,13 +1322,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1338,13 +1336,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1352,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1366,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1385,26 +1383,26 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1420,59 +1418,59 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+    <col min="12" max="12" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" t="s">
-        <v>98</v>
-      </c>
       <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1480,31 +1478,31 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1512,31 +1510,31 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1544,28 +1542,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1581,16 +1579,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -1599,37 +1597,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1645,21 +1643,21 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1667,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>